<commit_message>
feat: Add AbilityInfo loader
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/AbilityInfo.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/AbilityInfo.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
-  <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F803CC85-ACC6-4FF1-ABFD-96120646AB48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71846D50-C3FF-49A9-A3FF-404D7A766AAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{E2949BBB-A766-4786-82E2-6C450ECBE76F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{3B82CC8E-DC78-4041-956F-DD85B6D446B7}"/>
   </bookViews>
   <sheets>
     <sheet name="AbilityInfo" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
   <si>
     <t>key</t>
   </si>
@@ -33,6 +33,22 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Effect</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AbilityType</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxCount</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Price</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>int</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -40,6 +56,10 @@
     <t>string</t>
   </si>
   <si>
+    <t>Enum&lt;AbilityType&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -47,11 +67,7 @@
     <t>이름</t>
   </si>
   <si>
-    <t>AbilityType</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enum&lt;AbilityType&gt;</t>
+    <t>적용 수치</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -59,34 +75,25 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Effect</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>적용 수치</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MaxCount</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>최대 구매 횟수 제한</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Price</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>가격</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>모든 무기 공격력 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACharacter</t>
+  </si>
+  <si>
+    <t>최대 체력 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>방어력 증가</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -95,22 +102,18 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>모든 무기 공격력 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>장전 속도 증가</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>최대 체력 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>권총 공격력 증가</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>APistol</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>권총 집탄율 감소</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -123,6 +126,9 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>ARifle</t>
+  </si>
+  <si>
     <t>돌격소총 집탄율 감소</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -131,23 +137,94 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>샷건 공격력 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AShotgun</t>
+  </si>
+  <si>
+    <t>샷건 집탄율 감소</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>샷건 최대사거리 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>저격소총 공격력 증가</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>ASniper</t>
+  </si>
+  <si>
     <t>저격소총 최대사거리 증가</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>샷건 공격력 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>샷건 집탄율 감소</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>샷건 최대사거리 증가</t>
+    <t>기관단총 공격력 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMachinegun</t>
+  </si>
+  <si>
+    <t>기관단총 집탄율 감소</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>기관단총 최대사거리 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>런처 공격력 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALauncher</t>
+  </si>
+  <si>
+    <t>런처 공격 범위 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>런처 최대사거리 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>파편수류탄 공격력 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AConsumeItem</t>
+  </si>
+  <si>
+    <t>파편수류탄 공격 범위 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>냉기수류탄 공격력 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>냉기수류탄 공격 범위 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>냉기수류탄 냉기 지속시간 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMP수류탄 공격력 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMP수류탄 공격 범위 증가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMP수류탄 지속시간 증가</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -155,6 +232,9 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>AMonster</t>
+  </si>
+  <si>
     <t>일반 좀비에게 받는 피해 감소</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -172,90 +252,6 @@
   </si>
   <si>
     <t>보스 좀비에게 받는 피해 감소</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>파편수류탄 공격력 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>파편수류탄 공격 범위 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>기관단총 공격력 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>기관단총 집탄율 감소</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>기관단총 최대사거리 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>런처 공격력 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>런처 최대사거리 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>런처 공격 범위 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMP수류탄 공격력 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>냉기수류탄 냉기 지속시간 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>냉기수류탄 공격력 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>냉기수류탄 공격 범위 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMP수류탄 공격 범위 증가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACharacter</t>
-  </si>
-  <si>
-    <t>APistol</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ARifle</t>
-  </si>
-  <si>
-    <t>AShotgun</t>
-  </si>
-  <si>
-    <t>ASniper</t>
-  </si>
-  <si>
-    <t>AMachinegun</t>
-  </si>
-  <si>
-    <t>ALauncher</t>
-  </si>
-  <si>
-    <t>AConsumeItem</t>
-  </si>
-  <si>
-    <t>AMonster</t>
-  </si>
-  <si>
-    <t>EMP수류탄 지속시간 증가</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -263,7 +259,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,13 +291,6 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -326,41 +315,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="1" xr:uid="{4A28EE7D-A2EB-4FD0-8214-531E7F18D1F9}"/>
+    <cellStyle name="표준 2" xfId="1" xr:uid="{0DF8D82A-F22B-4375-AD16-B50300A3FE96}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -671,14 +645,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DA556D-28DB-488A-A027-DA59F239C317}">
-  <sheetPr codeName="Sheet5">
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:P42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43D6575-C278-4AD7-B764-40B71458748C}">
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -689,18 +660,9 @@
     <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,94 +670,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -803,23 +741,19 @@
       <c r="F4">
         <v>100</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -827,23 +761,19 @@
       <c r="F5">
         <v>100</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -851,23 +781,19 @@
       <c r="F6">
         <v>100</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -875,23 +801,19 @@
       <c r="F7">
         <v>100</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -899,13 +821,9 @@
       <c r="F8">
         <v>100</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>6</v>
       </c>
       <c r="B9" t="s">
@@ -915,7 +833,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -923,47 +841,39 @@
       <c r="F9">
         <v>100</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>7</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10">
         <v>100</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -971,26 +881,19 @@
       <c r="F11">
         <v>100</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -998,26 +901,19 @@
       <c r="F12">
         <v>100</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -1025,43 +921,29 @@
       <c r="F13">
         <v>100</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>11</v>
       </c>
       <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
         <v>26</v>
       </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <v>100</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>12</v>
       </c>
       <c r="B15" t="s">
@@ -1071,7 +953,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1079,26 +961,19 @@
       <c r="F15">
         <v>100</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1106,26 +981,19 @@
       <c r="F16">
         <v>100</v>
       </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -1133,26 +1001,19 @@
       <c r="F17">
         <v>100</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -1160,26 +1021,19 @@
       <c r="F18">
         <v>100</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -1187,26 +1041,19 @@
       <c r="F19">
         <v>100</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -1214,26 +1061,19 @@
       <c r="F20">
         <v>100</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -1241,26 +1081,19 @@
       <c r="F21">
         <v>100</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1268,21 +1101,19 @@
       <c r="F22">
         <v>100</v>
       </c>
-      <c r="J22" s="6"/>
-      <c r="M22" s="8"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -1290,21 +1121,19 @@
       <c r="F23">
         <v>100</v>
       </c>
-      <c r="J23" s="6"/>
-      <c r="M23" s="8"/>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -1312,43 +1141,39 @@
       <c r="F24">
         <v>100</v>
       </c>
-      <c r="J24" s="6"/>
-      <c r="M24" s="8"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
         <v>22</v>
       </c>
       <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
         <v>44</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25">
-        <v>100</v>
-      </c>
-      <c r="J25" s="6"/>
-      <c r="M25" s="8"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>23</v>
-      </c>
-      <c r="B26" t="s">
-        <v>38</v>
       </c>
       <c r="C26">
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -1356,21 +1181,19 @@
       <c r="F26">
         <v>100</v>
       </c>
-      <c r="J26" s="6"/>
-      <c r="M26" s="8"/>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -1378,21 +1201,19 @@
       <c r="F27">
         <v>100</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="M27" s="8"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -1401,38 +1222,38 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
         <v>26</v>
       </c>
       <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
         <v>49</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29">
-        <v>3</v>
-      </c>
-      <c r="F29">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
-        <v>27</v>
-      </c>
-      <c r="B30" t="s">
-        <v>47</v>
       </c>
       <c r="C30">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -1441,18 +1262,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C31">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -1461,18 +1282,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -1482,17 +1303,17 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
+      <c r="A33" s="3">
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C33">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -1502,17 +1323,17 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="A34" s="3">
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C34">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -1522,97 +1343,97 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
+      <c r="A35" s="3">
         <v>32</v>
       </c>
       <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="4">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
         <v>33</v>
       </c>
-      <c r="C35" s="7">
-        <v>3</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="4">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="4">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="4">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
         <v>59</v>
       </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
-      <c r="F35">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
-        <v>33</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="7">
+      <c r="C39" s="4">
         <v>7</v>
       </c>
-      <c r="D36" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36">
-        <v>3</v>
-      </c>
-      <c r="F36">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
-        <v>34</v>
-      </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="7">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
-        <v>35</v>
-      </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="7">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s">
-        <v>59</v>
-      </c>
-      <c r="E38">
-        <v>3</v>
-      </c>
-      <c r="F38">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
-        <v>36</v>
-      </c>
-      <c r="B39" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="7">
-        <v>7</v>
-      </c>
       <c r="D39" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E39">
         <v>2</v>
@@ -1620,20 +1441,9 @@
       <c r="F39">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>